<commit_message>
GMS Data Release 1
</commit_message>
<xml_diff>
--- a/DBFieldsDataType/Exomiser.xlsx
+++ b/DBFieldsDataType/Exomiser.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Labkey_DataReleases_V10\DBFieldsDataType\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\GMSLabkey\DBFieldsDataType\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E7EC785-5126-405E-BB4A-8030B3AE3FD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="42">
   <si>
     <t>key</t>
   </si>
@@ -35,9 +36,6 @@
     <t>participant_id</t>
   </si>
   <si>
-    <t>family_id</t>
-  </si>
-  <si>
     <t>character varying</t>
   </si>
   <si>
@@ -47,9 +45,6 @@
     <t>interpretation_request_id</t>
   </si>
   <si>
-    <t>sample_id</t>
-  </si>
-  <si>
     <t>phenotype</t>
   </si>
   <si>
@@ -59,9 +54,6 @@
     <t>participant_phenotypic_sex</t>
   </si>
   <si>
-    <t>assembly</t>
-  </si>
-  <si>
     <t>chromosome</t>
   </si>
   <si>
@@ -143,22 +135,28 @@
     <t>father_affected</t>
   </si>
   <si>
-    <t>full_brothers_affected</t>
-  </si>
-  <si>
-    <t>full_sisters_affected</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
     <t>Type</t>
+  </si>
+  <si>
+    <t>referral_id</t>
+  </si>
+  <si>
+    <t>full_siblings_affected</t>
+  </si>
+  <si>
+    <t>platekey</t>
+  </si>
+  <si>
+    <t>genome_build</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -515,28 +513,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1"/>
-    <col min="2" max="2" width="25.28515625" customWidth="1"/>
+    <col min="1" max="1" width="19.26953125" customWidth="1"/>
+    <col min="2" max="2" width="25.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -544,7 +542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -552,293 +550,289 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="B5" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="B6" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="B8" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="B9" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="B10" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="B12" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="B17" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="B18" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B23" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" s="2" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="B28" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+      <c r="B29" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+      <c r="B30" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+      <c r="B31" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+      <c r="B32" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+      <c r="B33" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+      <c r="B34" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+      <c r="B35" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
+      <c r="B36" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="B37" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>4</v>
-      </c>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>